<commit_message>
sync with xl, genesis block modification
</commit_message>
<xml_diff>
--- a/functions/ledger.xlsx
+++ b/functions/ledger.xlsx
@@ -1,76 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <fileSharing readOnlyRecommended="1" userName="Rakshit" algorithmName="SHA-512" hashValue="etzDEFSm3e7sP+uHC6YrAgc3RJPnQSFbyiqeUn98G03HTULSCH4jBnZL8Z5doXygbgRXdXjHc8U3GRweiN6E2w==" saltValue="6CrQ6VbBvGeUIFUJW/+53w==" spinCount="100000"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\CryPy\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10001_{B73729FD-5420-40AC-A171-E4DB7CF36723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6264" yWindow="1500" windowWidth="13416" windowHeight="8676" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5016" yWindow="2628" windowWidth="13416" windowHeight="8676" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Index</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>From</t>
-  </si>
-  <si>
-    <t>To</t>
-  </si>
-  <si>
-    <t>Event</t>
-  </si>
-  <si>
-    <t>Previous</t>
-  </si>
-  <si>
-    <t>Stringfied Details</t>
-  </si>
-  <si>
-    <t>Hash</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -89,22 +54,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -370,49 +394,109 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.109375" bestFit="1" customWidth="1"/>
+    <col width="5.6640625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="7.88671875" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="5.33203125" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="3.109375" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="8" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="8.21875" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="117.21875" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="5.109375" bestFit="1" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" customFormat="1" s="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Index</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>From</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>To</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Previous</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Stringfied Details</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Hash</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>spuckhafte_ferwirklung#7109</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2112202123</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0000000000000000000000000000000000000000000000000000000000000000</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1/1.0,?:spuckhafte_ferwirklung#7109(2112202123)/0000000000000000000000000000000000000000000000000000000000000000/20548364</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2005cc04ab531195369efaf51d292e7dfc50d76fe222ce468e3ec10d914a60a3</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new restrictions for transferring money
</commit_message>
<xml_diff>
--- a/functions/ledger.xlsx
+++ b/functions/ledger.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5016" yWindow="2628" windowWidth="13416" windowHeight="8676" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -399,10 +399,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A2" sqref="A2:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -414,7 +414,7 @@
     <col width="8" bestFit="1" customWidth="1" min="5" max="5"/>
     <col width="8.21875" bestFit="1" customWidth="1" min="6" max="6"/>
     <col width="117.21875" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="5.109375" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="65.21875" bestFit="1" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="1">
@@ -480,7 +480,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2112202123</t>
+          <t>231220212</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -490,12 +490,52 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1/1.0,?:spuckhafte_ferwirklung#7109(2112202123)/0000000000000000000000000000000000000000000000000000000000000000/20548364</t>
+          <t>1/1.0,?:spuckhafte_ferwirklung#7109(231220212)/0000000000000000000000000000000000000000000000000000000000000000/22489572/~~2005cce2777be4eb4c770fb377d4963b8a24b72ae10a43fd97aaeb33f8dfa5cb</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2005cc04ab531195369efaf51d292e7dfc50d76fe222ce468e3ec10d914a60a3</t>
+          <t>2005cce2777be4eb4c770fb377d4963b8a24b72ae10a43fd97aaeb33f8dfa5cb</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>spuckhafte_ferwirklung#7109</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Ayano#3463</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>231220212</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2005cce2777be4eb4c770fb377d4963b8a24b72ae10a43fd97aaeb33f8dfa5cb</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2/1,spuckhafte_ferwirklung#7109:Ayano#3463(231220212)/2005cce2777be4eb4c770fb377d4963b8a24b72ae10a43fd97aaeb33f8dfa5cb/15007020/~~2005cc034ce6dd8803c2bf65ad313694059dea96b43a5deda13fdfc8d2d61f6d</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2005cc034ce6dd8803c2bf65ad313694059dea96b43a5deda13fdfc8d2d61f6d</t>
         </is>
       </c>
     </row>

</xml_diff>